<commit_message>
August 25 pre-release updates
    Updated waste emissions calculation
    Fixed ordering of incorporation of user-added energy data
    Improved consistency of unit conversions throughout code
    India emissions now generally calibrated to GAINS emission factors
    USA emissions now scaled to most recent EPA Trends data
    Minimum transportation emission factor pathways updated
    Aggregate industrial sector emissions seasonality changed to flat for all countries
    Other code clean-up and improvements
</commit_message>
<xml_diff>
--- a/input/general/biomass_heat_content.xlsx
+++ b/input/general/biomass_heat_content.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Documents/Information &amp; Documents/CEDS_Project/CEDS/input/general/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9306D124-1069-F94A-93D2-78EDCE95B294}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5780" yWindow="-80" windowWidth="21600" windowHeight="13740" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="960" yWindow="460" windowWidth="21600" windowHeight="13740" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bio EF Calcs.xlsx" sheetId="1" r:id="rId1"/>
@@ -18,15 +24,21 @@
     <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
-    <definedName name="conv_toe_agwaste">[3]Conversions!$C$6</definedName>
-    <definedName name="conv_toe_charc">[3]Conversions!$C$3</definedName>
-    <definedName name="conv_toe_dung">[3]Conversions!$C$5</definedName>
-    <definedName name="conv_toe_fw">[3]Conversions!$C$4</definedName>
-    <definedName name="conv_toe_fw2">[4]Conversions!$C$4</definedName>
-    <definedName name="g">[4]Conversions!$C$4</definedName>
+    <definedName name="conv_toe_agwaste">[1]Conversions!$C$6</definedName>
+    <definedName name="conv_toe_charc">[1]Conversions!$C$3</definedName>
+    <definedName name="conv_toe_dung">[1]Conversions!$C$5</definedName>
+    <definedName name="conv_toe_fw">[1]Conversions!$C$4</definedName>
+    <definedName name="conv_toe_fw2">[2]Conversions!$C$4</definedName>
+    <definedName name="g">[2]Conversions!$C$4</definedName>
   </definedNames>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -35,12 +47,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>AndrewM</author>
   </authors>
   <commentList>
-    <comment ref="A54" authorId="0">
+    <comment ref="A54" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -69,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="100">
   <si>
     <t xml:space="preserve">According to the IEA, bagasse is included in industrial biofuel estimates.  Before we knew this, Suneeta calculated bagasse separately.  </t>
   </si>
@@ -418,21 +430,22 @@
   <si>
     <t>Bagasse</t>
   </si>
+  <si>
+    <t>MJ/kg</t>
+  </si>
+  <si>
+    <t>(Roughly equivalent to wood at ~23% water content - Wood Fuels Handbook - FAO (Krajnc 2015)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="0.0000"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -449,6 +462,7 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -475,6 +489,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
@@ -506,6 +521,10 @@
       <color indexed="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -664,7 +683,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -673,7 +692,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -706,8 +725,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -729,8 +748,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -739,17 +756,128 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Conversions"/>
+      <sheetName val="Pop"/>
+      <sheetName val="SPEW"/>
+      <sheetName val="Res_FW"/>
+      <sheetName val="Res_CC"/>
+      <sheetName val="Res_Ag Res"/>
+      <sheetName val="Res_Dung"/>
+      <sheetName val="FuelTotal"/>
+      <sheetName val="Sorting"/>
+      <sheetName val="FW Total"/>
+      <sheetName val="FW Ind"/>
+      <sheetName val="Bagasse"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1">
+        <row r="3">
+          <cell r="C3">
+            <v>1359.3506493506493</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="C4">
+            <v>3033.9130434782605</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="C5">
+            <v>330</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="C6">
+            <v>2791.2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Conversions"/>
+      <sheetName val="Observ"/>
+      <sheetName val="OneCountry"/>
+      <sheetName val="per_cap"/>
+      <sheetName val="per_cap_comp"/>
+      <sheetName val="forest_urban"/>
+      <sheetName val="solid"/>
+      <sheetName val="GDP"/>
+      <sheetName val="population"/>
+      <sheetName val="RWEDP"/>
+      <sheetName val="FAOStat"/>
+      <sheetName val="res_bio"/>
+      <sheetName val="res_coal"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="4">
+          <cell r="C4">
+            <v>3033.9130434782605</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Input Assumptions"/>
@@ -1203,8 +1331,8 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Legend"/>
@@ -1545,105 +1673,6 @@
       <sheetData sheetId="26"/>
       <sheetData sheetId="27"/>
       <sheetData sheetId="28"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Conversions"/>
-      <sheetName val="Pop"/>
-      <sheetName val="SPEW"/>
-      <sheetName val="Res_FW"/>
-      <sheetName val="Res_CC"/>
-      <sheetName val="Res_Ag Res"/>
-      <sheetName val="Res_Dung"/>
-      <sheetName val="FuelTotal"/>
-      <sheetName val="Sorting"/>
-      <sheetName val="FW Total"/>
-      <sheetName val="FW Ind"/>
-      <sheetName val="Bagasse"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1">
-        <row r="3">
-          <cell r="C3">
-            <v>1359.3506493506493</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="C4">
-            <v>3033.9130434782605</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="C5">
-            <v>330</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="C6">
-            <v>2791.2</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Conversions"/>
-      <sheetName val="Observ"/>
-      <sheetName val="OneCountry"/>
-      <sheetName val="per_cap"/>
-      <sheetName val="per_cap_comp"/>
-      <sheetName val="forest_urban"/>
-      <sheetName val="solid"/>
-      <sheetName val="GDP"/>
-      <sheetName val="population"/>
-      <sheetName val="RWEDP"/>
-      <sheetName val="FAOStat"/>
-      <sheetName val="res_bio"/>
-      <sheetName val="res_coal"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="4">
-          <cell r="C4">
-            <v>3033.9130434782605</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1968,15 +1997,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K2" sqref="K2:K6"/>
+      <selection pane="topRight" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.83203125" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" customWidth="1"/>
@@ -1989,12 +2018,12 @@
     <col min="9" max="9" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -2018,7 +2047,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>43</v>
       </c>
@@ -2039,11 +2068,11 @@
         <v>47</v>
       </c>
       <c r="K3" s="26">
-        <f>C3*10^6*2.388458966275*10^(-8)</f>
-        <v>0.38215343460400003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <f>C3*(10^6)/42*10^(-6)</f>
+        <v>0.38095238095238093</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>48</v>
       </c>
@@ -2064,11 +2093,11 @@
         <v>50</v>
       </c>
       <c r="K4" s="26">
-        <f t="shared" ref="K4:K6" si="0">C4*10^6*2.388458966275*10^(-8)</f>
-        <v>0.32244196044712498</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <f t="shared" ref="K4:K6" si="0">C4*(10^6)/42*10^(-6)</f>
+        <v>0.3214285714285714</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>51</v>
       </c>
@@ -2090,10 +2119,10 @@
       </c>
       <c r="K5" s="26">
         <f t="shared" si="0"/>
-        <v>0.34632655010987501</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>0.34523809523809523</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>53</v>
       </c>
@@ -2115,10 +2144,10 @@
       </c>
       <c r="K6" s="26">
         <f t="shared" si="0"/>
-        <v>0.57323015190600002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>0.57142857142857151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>57</v>
       </c>
@@ -2129,7 +2158,7 @@
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>37</v>
       </c>
@@ -2157,7 +2186,7 @@
       </c>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>60</v>
       </c>
@@ -2187,7 +2216,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>64</v>
       </c>
@@ -2217,7 +2246,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>53</v>
       </c>
@@ -2240,7 +2269,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>60</v>
       </c>
@@ -2270,7 +2299,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>64</v>
       </c>
@@ -2300,7 +2329,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>48</v>
       </c>
@@ -2323,7 +2352,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>51</v>
       </c>
@@ -2346,12 +2375,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B19" s="1"/>
       <c r="C19" s="13" t="str">
         <f>$B$10</f>
@@ -2382,7 +2411,7 @@
         <v>traditional</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="17" customFormat="1">
+    <row r="20" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
         <v>71</v>
       </c>
@@ -2422,7 +2451,7 @@
       </c>
       <c r="K20" s="13"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>73</v>
       </c>
@@ -2461,7 +2490,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -2500,7 +2529,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>75</v>
       </c>
@@ -2539,7 +2568,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>76</v>
       </c>
@@ -2578,7 +2607,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>77</v>
       </c>
@@ -2617,7 +2646,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>78</v>
       </c>
@@ -2656,7 +2685,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>79</v>
       </c>
@@ -2695,7 +2724,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>80</v>
       </c>
@@ -2734,7 +2763,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>81</v>
       </c>
@@ -2773,7 +2802,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>82</v>
       </c>
@@ -2812,7 +2841,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>83</v>
       </c>
@@ -2851,7 +2880,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>84</v>
       </c>
@@ -2890,7 +2919,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>85</v>
       </c>
@@ -2929,7 +2958,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>86</v>
       </c>
@@ -2968,12 +2997,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B37" s="1"/>
       <c r="C37" s="13" t="str">
         <f>$C$19</f>
@@ -2996,7 +3025,7 @@
         <v>traditional</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="15" t="s">
         <v>71</v>
       </c>
@@ -3027,7 +3056,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>73</v>
       </c>
@@ -3035,7 +3064,7 @@
         <v>49</v>
       </c>
       <c r="C39" s="9" t="str">
-        <f>IF($B39="Commercial",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A39,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B39="Commercial",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A39,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v/>
       </c>
       <c r="D39" s="18">
@@ -3043,7 +3072,7 @@
         <v>1</v>
       </c>
       <c r="E39" s="9">
-        <f>IF($B39="Traditional",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A39,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B39="Traditional",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A39,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v>0.7406858003484933</v>
       </c>
       <c r="F39" s="9">
@@ -3058,7 +3087,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>74</v>
       </c>
@@ -3066,7 +3095,7 @@
         <v>54</v>
       </c>
       <c r="C40" s="9">
-        <f>IF($B40="Commercial",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A40,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B40="Commercial",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A40,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v>1.35</v>
       </c>
       <c r="D40" s="18">
@@ -3074,7 +3103,7 @@
         <v>1</v>
       </c>
       <c r="E40" s="9" t="str">
-        <f>IF($B40="Traditional",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A40,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B40="Traditional",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A40,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v/>
       </c>
       <c r="F40" s="9" t="str">
@@ -3089,7 +3118,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>75</v>
       </c>
@@ -3097,7 +3126,7 @@
         <v>54</v>
       </c>
       <c r="C41" s="9">
-        <f>IF($B41="Commercial",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A41,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B41="Commercial",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A41,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v>1.35</v>
       </c>
       <c r="D41" s="18">
@@ -3105,7 +3134,7 @@
         <v>1</v>
       </c>
       <c r="E41" s="9" t="str">
-        <f>IF($B41="Traditional",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A41,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B41="Traditional",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A41,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v/>
       </c>
       <c r="F41" s="9" t="str">
@@ -3120,7 +3149,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>76</v>
       </c>
@@ -3128,7 +3157,7 @@
         <v>49</v>
       </c>
       <c r="C42" s="9" t="str">
-        <f>IF($B42="Commercial",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A42,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B42="Commercial",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A42,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v/>
       </c>
       <c r="D42" s="18">
@@ -3136,7 +3165,7 @@
         <v>1</v>
       </c>
       <c r="E42" s="9">
-        <f>IF($B42="Traditional",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A42,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B42="Traditional",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A42,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v>1.0040069406275216</v>
       </c>
       <c r="F42" s="9">
@@ -3151,7 +3180,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>77</v>
       </c>
@@ -3159,7 +3188,7 @@
         <v>54</v>
       </c>
       <c r="C43" s="9">
-        <f>IF($B43="Commercial",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A43,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B43="Commercial",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A43,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v>1.35</v>
       </c>
       <c r="D43" s="18">
@@ -3167,7 +3196,7 @@
         <v>1</v>
       </c>
       <c r="E43" s="9" t="str">
-        <f>IF($B43="Traditional",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A43,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B43="Traditional",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A43,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v/>
       </c>
       <c r="F43" s="9" t="str">
@@ -3182,7 +3211,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>78</v>
       </c>
@@ -3190,7 +3219,7 @@
         <v>54</v>
       </c>
       <c r="C44" s="9">
-        <f>IF($B44="Commercial",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A44,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B44="Commercial",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A44,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v>1.35</v>
       </c>
       <c r="D44" s="18">
@@ -3198,7 +3227,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="9" t="str">
-        <f>IF($B44="Traditional",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A44,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B44="Traditional",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A44,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v/>
       </c>
       <c r="F44" s="9" t="str">
@@ -3213,7 +3242,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>79</v>
       </c>
@@ -3221,7 +3250,7 @@
         <v>49</v>
       </c>
       <c r="C45" s="9" t="str">
-        <f>IF($B45="Commercial",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A45,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B45="Commercial",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A45,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v/>
       </c>
       <c r="D45" s="18">
@@ -3229,7 +3258,7 @@
         <v>1</v>
       </c>
       <c r="E45" s="9">
-        <f>IF($B45="Traditional",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A45,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B45="Traditional",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A45,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v>0.70082430010607955</v>
       </c>
       <c r="F45" s="9">
@@ -3244,7 +3273,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>80</v>
       </c>
@@ -3252,7 +3281,7 @@
         <v>54</v>
       </c>
       <c r="C46" s="9">
-        <f>IF($B46="Commercial",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A46,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B46="Commercial",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A46,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v>1.35</v>
       </c>
       <c r="D46" s="18">
@@ -3260,7 +3289,7 @@
         <v>1</v>
       </c>
       <c r="E46" s="9" t="str">
-        <f>IF($B46="Traditional",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A46,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B46="Traditional",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A46,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v/>
       </c>
       <c r="F46" s="9" t="str">
@@ -3275,7 +3304,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>81</v>
       </c>
@@ -3283,7 +3312,7 @@
         <v>54</v>
       </c>
       <c r="C47" s="9">
-        <f>IF($B47="Commercial",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A47,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B47="Commercial",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A47,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v>1.35</v>
       </c>
       <c r="D47" s="18">
@@ -3291,7 +3320,7 @@
         <v>1</v>
       </c>
       <c r="E47" s="9" t="str">
-        <f>IF($B47="Traditional",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A47,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B47="Traditional",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A47,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v/>
       </c>
       <c r="F47" s="19">
@@ -3306,7 +3335,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>82</v>
       </c>
@@ -3314,7 +3343,7 @@
         <v>49</v>
       </c>
       <c r="C48" s="9" t="str">
-        <f>IF($B48="Commercial",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A48,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B48="Commercial",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A48,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v/>
       </c>
       <c r="D48" s="18">
@@ -3322,7 +3351,7 @@
         <v>1</v>
       </c>
       <c r="E48" s="9">
-        <f>IF($B48="Traditional",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A48,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B48="Traditional",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A48,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v>0.96287841902515781</v>
       </c>
       <c r="F48" s="9">
@@ -3337,7 +3366,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>83</v>
       </c>
@@ -3345,7 +3374,7 @@
         <v>54</v>
       </c>
       <c r="C49" s="9">
-        <f>IF($B49="Commercial",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A49,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B49="Commercial",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A49,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v>0.41</v>
       </c>
       <c r="D49" s="18">
@@ -3353,7 +3382,7 @@
         <v>1</v>
       </c>
       <c r="E49" s="9" t="str">
-        <f>IF($B49="Traditional",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A49,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B49="Traditional",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A49,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v/>
       </c>
       <c r="F49" s="9" t="str">
@@ -3368,7 +3397,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>84</v>
       </c>
@@ -3376,7 +3405,7 @@
         <v>49</v>
       </c>
       <c r="C50" s="9" t="str">
-        <f>IF($B50="Commercial",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A50,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B50="Commercial",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A50,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v/>
       </c>
       <c r="D50" s="18">
@@ -3384,7 +3413,7 @@
         <v>1</v>
       </c>
       <c r="E50" s="9">
-        <f>IF($B50="Traditional",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A50,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B50="Traditional",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A50,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v>0.71535921826132054</v>
       </c>
       <c r="F50" s="9">
@@ -3399,7 +3428,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>85</v>
       </c>
@@ -3407,7 +3436,7 @@
         <v>54</v>
       </c>
       <c r="C51" s="9">
-        <f>IF($B51="Commercial",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A51,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B51="Commercial",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A51,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v>1.35</v>
       </c>
       <c r="D51" s="18">
@@ -3415,7 +3444,7 @@
         <v>1</v>
       </c>
       <c r="E51" s="9" t="str">
-        <f>IF($B51="Traditional",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A51,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B51="Traditional",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A51,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v/>
       </c>
       <c r="F51" s="9" t="str">
@@ -3430,7 +3459,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>86</v>
       </c>
@@ -3438,7 +3467,7 @@
         <v>54</v>
       </c>
       <c r="C52" s="9">
-        <f>IF($B52="Commercial",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A52,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B52="Commercial",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A52,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v>1.35</v>
       </c>
       <c r="D52" s="18">
@@ -3446,7 +3475,7 @@
         <v>1</v>
       </c>
       <c r="E52" s="9" t="str">
-        <f>IF($B52="Traditional",INDEX('[1]Wood Split'!$F$5:$F$18,MATCH($A52,'[1]Wood Split'!$A$5:$A$18,0)),"")</f>
+        <f>IF($B52="Traditional",INDEX('[3]Wood Split'!$F$5:$F$18,MATCH($A52,'[3]Wood Split'!$A$5:$A$18,0)),"")</f>
         <v/>
       </c>
       <c r="F52" s="9" t="str">
@@ -3461,12 +3490,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="15" t="s">
         <v>71</v>
       </c>
@@ -3478,7 +3507,7 @@
       </c>
       <c r="D55" s="20"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="21" t="s">
         <v>91</v>
       </c>
@@ -3486,203 +3515,203 @@
       <c r="C56" s="22"/>
       <c r="D56" s="20"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>73</v>
       </c>
       <c r="B57" s="23">
-        <f>INDEX('[1]Final Biomass EFs'!$K$4:$K$18,MATCH($A57,'[1]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([2]BC_calcs!$D$84:$Q$84,1,MATCH($A57,[2]BC_calcs!$D$55:$Q$55,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$4:$K$18,MATCH($A57,'[3]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([4]BC_calcs!$D$84:$Q$84,1,MATCH($A57,[4]BC_calcs!$D$55:$Q$55,0))</f>
         <v>3.7558480609715728E-2</v>
       </c>
       <c r="C57" s="24">
-        <f>INDEX('[1]Final Biomass EFs'!$K$30:$K$44,MATCH($A57,'[1]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([2]OC_calcs!$D$86:$Q$86,1,MATCH($A57,[2]OC_calcs!$D$56:$Q$56,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$30:$K$44,MATCH($A57,'[3]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([4]OC_calcs!$D$86:$Q$86,1,MATCH($A57,[4]OC_calcs!$D$56:$Q$56,0))</f>
         <v>5.0788172422917797E-2</v>
       </c>
       <c r="D57" s="20"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>74</v>
       </c>
       <c r="B58" s="23">
-        <f>INDEX('[1]Final Biomass EFs'!$K$4:$K$18,MATCH($A58,'[1]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([2]BC_calcs!$D$84:$Q$84,1,MATCH($A58,[2]BC_calcs!$D$55:$Q$55,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$4:$K$18,MATCH($A58,'[3]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([4]BC_calcs!$D$84:$Q$84,1,MATCH($A58,[4]BC_calcs!$D$55:$Q$55,0))</f>
         <v>3.4420610961357549E-3</v>
       </c>
       <c r="C58" s="24">
-        <f>INDEX('[1]Final Biomass EFs'!$K$30:$K$44,MATCH($A58,'[1]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([2]OC_calcs!$D$86:$Q$86,1,MATCH($A58,[2]OC_calcs!$D$56:$Q$56,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$30:$K$44,MATCH($A58,'[3]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([4]OC_calcs!$D$86:$Q$86,1,MATCH($A58,[4]OC_calcs!$D$56:$Q$56,0))</f>
         <v>1.1056900169151168E-2</v>
       </c>
       <c r="D58" s="20"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>75</v>
       </c>
       <c r="B59" s="23">
-        <f>INDEX('[1]Final Biomass EFs'!$K$4:$K$18,MATCH($A59,'[1]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([2]BC_calcs!$D$84:$Q$84,1,MATCH($A59,[2]BC_calcs!$D$55:$Q$55,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$4:$K$18,MATCH($A59,'[3]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([4]BC_calcs!$D$84:$Q$84,1,MATCH($A59,[4]BC_calcs!$D$55:$Q$55,0))</f>
         <v>6.773189086731763E-3</v>
       </c>
       <c r="C59" s="24">
-        <f>INDEX('[1]Final Biomass EFs'!$K$30:$K$44,MATCH($A59,'[1]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([2]OC_calcs!$D$86:$Q$86,1,MATCH($A59,[2]OC_calcs!$D$56:$Q$56,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$30:$K$44,MATCH($A59,'[3]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([4]OC_calcs!$D$86:$Q$86,1,MATCH($A59,[4]OC_calcs!$D$56:$Q$56,0))</f>
         <v>3.7439590257036179E-2</v>
       </c>
       <c r="D59" s="20"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>76</v>
       </c>
       <c r="B60" s="23">
-        <f>INDEX('[1]Final Biomass EFs'!$K$4:$K$18,MATCH($A60,'[1]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([2]BC_calcs!$D$84:$Q$84,1,MATCH($A60,[2]BC_calcs!$D$55:$Q$55,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$4:$K$18,MATCH($A60,'[3]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([4]BC_calcs!$D$84:$Q$84,1,MATCH($A60,[4]BC_calcs!$D$55:$Q$55,0))</f>
         <v>1.7437457740845327E-3</v>
       </c>
       <c r="C60" s="24">
-        <f>INDEX('[1]Final Biomass EFs'!$K$30:$K$44,MATCH($A60,'[1]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([2]OC_calcs!$D$86:$Q$86,1,MATCH($A60,[2]OC_calcs!$D$56:$Q$56,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$30:$K$44,MATCH($A60,'[3]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([4]OC_calcs!$D$86:$Q$86,1,MATCH($A60,[4]OC_calcs!$D$56:$Q$56,0))</f>
         <v>1.8659572797351711E-3</v>
       </c>
       <c r="D60" s="20"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>77</v>
       </c>
       <c r="B61" s="23">
-        <f>INDEX('[1]Final Biomass EFs'!$K$4:$K$18,MATCH($A61,'[1]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([2]BC_calcs!$D$84:$Q$84,1,MATCH($A61,[2]BC_calcs!$D$55:$Q$55,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$4:$K$18,MATCH($A61,'[3]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([4]BC_calcs!$D$84:$Q$84,1,MATCH($A61,[4]BC_calcs!$D$55:$Q$55,0))</f>
         <v>2.4873530944262319E-2</v>
       </c>
       <c r="C61" s="24">
-        <f>INDEX('[1]Final Biomass EFs'!$K$30:$K$44,MATCH($A61,'[1]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([2]OC_calcs!$D$86:$Q$86,1,MATCH($A61,[2]OC_calcs!$D$56:$Q$56,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$30:$K$44,MATCH($A61,'[3]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([4]OC_calcs!$D$86:$Q$86,1,MATCH($A61,[4]OC_calcs!$D$56:$Q$56,0))</f>
         <v>0.14551744905646391</v>
       </c>
       <c r="D61" s="20"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>78</v>
       </c>
       <c r="B62" s="23">
-        <f>INDEX('[1]Final Biomass EFs'!$K$4:$K$18,MATCH($A62,'[1]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([2]BC_calcs!$D$84:$Q$84,1,MATCH($A62,[2]BC_calcs!$D$55:$Q$55,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$4:$K$18,MATCH($A62,'[3]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([4]BC_calcs!$D$84:$Q$84,1,MATCH($A62,[4]BC_calcs!$D$55:$Q$55,0))</f>
         <v>2.2592900857125123E-2</v>
       </c>
       <c r="C62" s="24">
-        <f>INDEX('[1]Final Biomass EFs'!$K$30:$K$44,MATCH($A62,'[1]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([2]OC_calcs!$D$86:$Q$86,1,MATCH($A62,[2]OC_calcs!$D$56:$Q$56,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$30:$K$44,MATCH($A62,'[3]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([4]OC_calcs!$D$86:$Q$86,1,MATCH($A62,[4]OC_calcs!$D$56:$Q$56,0))</f>
         <v>0.13184464398494755</v>
       </c>
       <c r="D62" s="20"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>79</v>
       </c>
       <c r="B63" s="23">
-        <f>INDEX('[1]Final Biomass EFs'!$K$4:$K$18,MATCH($A63,'[1]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([2]BC_calcs!$D$84:$Q$84,1,MATCH($A63,[2]BC_calcs!$D$55:$Q$55,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$4:$K$18,MATCH($A63,'[3]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([4]BC_calcs!$D$84:$Q$84,1,MATCH($A63,[4]BC_calcs!$D$55:$Q$55,0))</f>
         <v>8.0761745347182161E-3</v>
       </c>
       <c r="C63" s="24">
-        <f>INDEX('[1]Final Biomass EFs'!$K$30:$K$44,MATCH($A63,'[1]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([2]OC_calcs!$D$86:$Q$86,1,MATCH($A63,[2]OC_calcs!$D$56:$Q$56,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$30:$K$44,MATCH($A63,'[3]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([4]OC_calcs!$D$86:$Q$86,1,MATCH($A63,[4]OC_calcs!$D$56:$Q$56,0))</f>
         <v>1.2319388467807975E-2</v>
       </c>
       <c r="D63" s="20"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>80</v>
       </c>
       <c r="B64" s="23">
-        <f>INDEX('[1]Final Biomass EFs'!$K$4:$K$18,MATCH($A64,'[1]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([2]BC_calcs!$D$84:$Q$84,1,MATCH($A64,[2]BC_calcs!$D$55:$Q$55,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$4:$K$18,MATCH($A64,'[3]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([4]BC_calcs!$D$84:$Q$84,1,MATCH($A64,[4]BC_calcs!$D$55:$Q$55,0))</f>
         <v>5.9685917613247575E-6</v>
       </c>
       <c r="C64" s="24">
-        <f>INDEX('[1]Final Biomass EFs'!$K$30:$K$44,MATCH($A64,'[1]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([2]OC_calcs!$D$86:$Q$86,1,MATCH($A64,[2]OC_calcs!$D$56:$Q$56,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$30:$K$44,MATCH($A64,'[3]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([4]OC_calcs!$D$86:$Q$86,1,MATCH($A64,[4]OC_calcs!$D$56:$Q$56,0))</f>
         <v>5.9685917613247575E-6</v>
       </c>
       <c r="D64" s="20"/>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>81</v>
       </c>
       <c r="B65" s="23">
-        <f>INDEX('[1]Final Biomass EFs'!$K$4:$K$18,MATCH($A65,'[1]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([2]BC_calcs!$D$84:$Q$84,1,MATCH($A65,[2]BC_calcs!$D$55:$Q$55,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$4:$K$18,MATCH($A65,'[3]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([4]BC_calcs!$D$84:$Q$84,1,MATCH($A65,[4]BC_calcs!$D$55:$Q$55,0))</f>
         <v>1.0046618339639201E-3</v>
       </c>
       <c r="C65" s="24">
-        <f>INDEX('[1]Final Biomass EFs'!$K$30:$K$44,MATCH($A65,'[1]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([2]OC_calcs!$D$86:$Q$86,1,MATCH($A65,[2]OC_calcs!$D$56:$Q$56,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$30:$K$44,MATCH($A65,'[3]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([4]OC_calcs!$D$86:$Q$86,1,MATCH($A65,[4]OC_calcs!$D$56:$Q$56,0))</f>
         <v>6.411715643132177E-3</v>
       </c>
       <c r="D65" s="20"/>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>82</v>
       </c>
       <c r="B66" s="23">
-        <f>INDEX('[1]Final Biomass EFs'!$K$4:$K$18,MATCH($A66,'[1]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([2]BC_calcs!$D$84:$Q$84,1,MATCH($A66,[2]BC_calcs!$D$55:$Q$55,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$4:$K$18,MATCH($A66,'[3]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([4]BC_calcs!$D$84:$Q$84,1,MATCH($A66,[4]BC_calcs!$D$55:$Q$55,0))</f>
         <v>2.3140468987578101E-3</v>
       </c>
       <c r="C66" s="24">
-        <f>INDEX('[1]Final Biomass EFs'!$K$30:$K$44,MATCH($A66,'[1]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([2]OC_calcs!$D$86:$Q$86,1,MATCH($A66,[2]OC_calcs!$D$56:$Q$56,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$30:$K$44,MATCH($A66,'[3]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([4]OC_calcs!$D$86:$Q$86,1,MATCH($A66,[4]OC_calcs!$D$56:$Q$56,0))</f>
         <v>2.3536799778386564E-3</v>
       </c>
       <c r="D66" s="20"/>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>83</v>
       </c>
       <c r="B67" s="23">
-        <f>INDEX('[1]Final Biomass EFs'!$K$4:$K$18,MATCH($A67,'[1]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([2]BC_calcs!$D$84:$Q$84,1,MATCH($A67,[2]BC_calcs!$D$55:$Q$55,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$4:$K$18,MATCH($A67,'[3]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([4]BC_calcs!$D$84:$Q$84,1,MATCH($A67,[4]BC_calcs!$D$55:$Q$55,0))</f>
         <v>2.0112841240392263E-3</v>
       </c>
       <c r="C67" s="24">
-        <f>INDEX('[1]Final Biomass EFs'!$K$30:$K$44,MATCH($A67,'[1]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([2]OC_calcs!$D$86:$Q$86,1,MATCH($A67,[2]OC_calcs!$D$56:$Q$56,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$30:$K$44,MATCH($A67,'[3]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([4]OC_calcs!$D$86:$Q$86,1,MATCH($A67,[4]OC_calcs!$D$56:$Q$56,0))</f>
         <v>3.016926186058839E-3</v>
       </c>
       <c r="D67" s="20"/>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>84</v>
       </c>
       <c r="B68" s="23">
-        <f>INDEX('[1]Final Biomass EFs'!$K$4:$K$18,MATCH($A68,'[1]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([2]BC_calcs!$D$84:$Q$84,1,MATCH($A68,[2]BC_calcs!$D$55:$Q$55,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$4:$K$18,MATCH($A68,'[3]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([4]BC_calcs!$D$84:$Q$84,1,MATCH($A68,[4]BC_calcs!$D$55:$Q$55,0))</f>
         <v>9.6286306294891561E-3</v>
       </c>
       <c r="C68" s="24">
-        <f>INDEX('[1]Final Biomass EFs'!$K$30:$K$44,MATCH($A68,'[1]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([2]OC_calcs!$D$86:$Q$86,1,MATCH($A68,[2]OC_calcs!$D$56:$Q$56,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$30:$K$44,MATCH($A68,'[3]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([4]OC_calcs!$D$86:$Q$86,1,MATCH($A68,[4]OC_calcs!$D$56:$Q$56,0))</f>
         <v>1.3732639570416391E-2</v>
       </c>
       <c r="D68" s="20"/>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>85</v>
       </c>
       <c r="B69" s="23">
-        <f>INDEX('[1]Final Biomass EFs'!$K$4:$K$18,MATCH($A69,'[1]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([2]BC_calcs!$D$84:$Q$84,1,MATCH($A69,[2]BC_calcs!$D$55:$Q$55,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$4:$K$18,MATCH($A69,'[3]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([4]BC_calcs!$D$84:$Q$84,1,MATCH($A69,[4]BC_calcs!$D$55:$Q$55,0))</f>
         <v>4.8118927301521869E-2</v>
       </c>
       <c r="C69" s="24">
-        <f>INDEX('[1]Final Biomass EFs'!$K$30:$K$44,MATCH($A69,'[1]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([2]OC_calcs!$D$86:$Q$86,1,MATCH($A69,[2]OC_calcs!$D$56:$Q$56,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$30:$K$44,MATCH($A69,'[3]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([4]OC_calcs!$D$86:$Q$86,1,MATCH($A69,[4]OC_calcs!$D$56:$Q$56,0))</f>
         <v>0.26607390448505985</v>
       </c>
       <c r="D69" s="20"/>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>86</v>
       </c>
       <c r="B70" s="23">
-        <f>INDEX('[1]Final Biomass EFs'!$K$4:$K$18,MATCH($A70,'[1]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([2]BC_calcs!$D$84:$Q$84,1,MATCH($A70,[2]BC_calcs!$D$55:$Q$55,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$4:$K$18,MATCH($A70,'[3]Final Biomass EFs'!$A$4:$A$18,0))*INDEX([4]BC_calcs!$D$84:$Q$84,1,MATCH($A70,[4]BC_calcs!$D$55:$Q$55,0))</f>
         <v>4.6618126935899118E-2</v>
       </c>
       <c r="C70" s="24">
-        <f>INDEX('[1]Final Biomass EFs'!$K$30:$K$44,MATCH($A70,'[1]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([2]OC_calcs!$D$86:$Q$86,1,MATCH($A70,[2]OC_calcs!$D$56:$Q$56,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$30:$K$44,MATCH($A70,'[3]Final Biomass EFs'!$A$30:$A$44,0))*INDEX([4]OC_calcs!$D$86:$Q$86,1,MATCH($A70,[4]OC_calcs!$D$56:$Q$56,0))</f>
         <v>0.21955932944561632</v>
       </c>
       <c r="D70" s="20"/>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="21" t="s">
         <v>92</v>
       </c>
@@ -3690,72 +3719,72 @@
       <c r="C71" s="22"/>
       <c r="D71" s="20"/>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>73</v>
       </c>
       <c r="B72" s="23">
-        <f>INDEX('[1]Final Biomass EFs'!$K$22:$K$26,MATCH($A72,'[1]Final Biomass EFs'!$A$22:$A$26,0))*INDEX([2]BC_calcs!$D$86:$Q$86,1,MATCH($A72,[2]BC_calcs!$D$55:$Q$55,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$22:$K$26,MATCH($A72,'[3]Final Biomass EFs'!$A$22:$A$26,0))*INDEX([4]BC_calcs!$D$86:$Q$86,1,MATCH($A72,[4]BC_calcs!$D$55:$Q$55,0))</f>
         <v>0.25876208442879295</v>
       </c>
       <c r="C72" s="24">
-        <f>INDEX('[1]Final Biomass EFs'!$K$48:$K$52,MATCH($A72,'[1]Final Biomass EFs'!$A$48:$A$52,0))*INDEX([2]OC_calcs!$D$88:$Q$88,1,MATCH($A72,[2]OC_calcs!$D$56:$Q$56,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$48:$K$52,MATCH($A72,'[3]Final Biomass EFs'!$A$48:$A$52,0))*INDEX([4]OC_calcs!$D$88:$Q$88,1,MATCH($A72,[4]OC_calcs!$D$56:$Q$56,0))</f>
         <v>0.90719227203529829</v>
       </c>
       <c r="D72" s="20"/>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>76</v>
       </c>
       <c r="B73" s="23">
-        <f>INDEX('[1]Final Biomass EFs'!$K$22:$K$26,MATCH($A73,'[1]Final Biomass EFs'!$A$22:$A$26,0))*INDEX([2]BC_calcs!$D$86:$Q$86,1,MATCH($A73,[2]BC_calcs!$D$55:$Q$55,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$22:$K$26,MATCH($A73,'[3]Final Biomass EFs'!$A$22:$A$26,0))*INDEX([4]BC_calcs!$D$86:$Q$86,1,MATCH($A73,[4]BC_calcs!$D$55:$Q$55,0))</f>
         <v>0.44395659685980143</v>
       </c>
       <c r="C73" s="24">
-        <f>INDEX('[1]Final Biomass EFs'!$K$48:$K$52,MATCH($A73,'[1]Final Biomass EFs'!$A$48:$A$52,0))*INDEX([2]OC_calcs!$D$88:$Q$88,1,MATCH($A73,[2]OC_calcs!$D$56:$Q$56,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$48:$K$52,MATCH($A73,'[3]Final Biomass EFs'!$A$48:$A$52,0))*INDEX([4]OC_calcs!$D$88:$Q$88,1,MATCH($A73,[4]OC_calcs!$D$56:$Q$56,0))</f>
         <v>1.5715151393598035</v>
       </c>
       <c r="D73" s="20"/>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>79</v>
       </c>
       <c r="B74" s="23">
-        <f>INDEX('[1]Final Biomass EFs'!$K$22:$K$26,MATCH($A74,'[1]Final Biomass EFs'!$A$22:$A$26,0))*INDEX([2]BC_calcs!$D$86:$Q$86,1,MATCH($A74,[2]BC_calcs!$D$55:$Q$55,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$22:$K$26,MATCH($A74,'[3]Final Biomass EFs'!$A$22:$A$26,0))*INDEX([4]BC_calcs!$D$86:$Q$86,1,MATCH($A74,[4]BC_calcs!$D$55:$Q$55,0))</f>
         <v>0.19453096774151155</v>
       </c>
       <c r="C74" s="24">
-        <f>INDEX('[1]Final Biomass EFs'!$K$48:$K$52,MATCH($A74,'[1]Final Biomass EFs'!$A$48:$A$52,0))*INDEX([2]OC_calcs!$D$88:$Q$88,1,MATCH($A74,[2]OC_calcs!$D$56:$Q$56,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$48:$K$52,MATCH($A74,'[3]Final Biomass EFs'!$A$48:$A$52,0))*INDEX([4]OC_calcs!$D$88:$Q$88,1,MATCH($A74,[4]OC_calcs!$D$56:$Q$56,0))</f>
         <v>0.71768688472266051</v>
       </c>
       <c r="D74" s="20"/>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>82</v>
       </c>
       <c r="B75" s="23">
-        <f>INDEX('[1]Final Biomass EFs'!$K$22:$K$26,MATCH($A75,'[1]Final Biomass EFs'!$A$22:$A$26,0))*INDEX([2]BC_calcs!$D$86:$Q$86,1,MATCH($A75,[2]BC_calcs!$D$55:$Q$55,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$22:$K$26,MATCH($A75,'[3]Final Biomass EFs'!$A$22:$A$26,0))*INDEX([4]BC_calcs!$D$86:$Q$86,1,MATCH($A75,[4]BC_calcs!$D$55:$Q$55,0))</f>
         <v>4.6067182706932719E-2</v>
       </c>
       <c r="C75" s="24">
-        <f>INDEX('[1]Final Biomass EFs'!$K$48:$K$52,MATCH($A75,'[1]Final Biomass EFs'!$A$48:$A$52,0))*INDEX([2]OC_calcs!$D$88:$Q$88,1,MATCH($A75,[2]OC_calcs!$D$56:$Q$56,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$48:$K$52,MATCH($A75,'[3]Final Biomass EFs'!$A$48:$A$52,0))*INDEX([4]OC_calcs!$D$88:$Q$88,1,MATCH($A75,[4]OC_calcs!$D$56:$Q$56,0))</f>
         <v>0.17722483169932099</v>
       </c>
       <c r="D75" s="20"/>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>84</v>
       </c>
       <c r="B76" s="23">
-        <f>INDEX('[1]Final Biomass EFs'!$K$22:$K$26,MATCH($A76,'[1]Final Biomass EFs'!$A$22:$A$26,0))*INDEX([2]BC_calcs!$D$86:$Q$86,1,MATCH($A76,[2]BC_calcs!$D$55:$Q$55,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$22:$K$26,MATCH($A76,'[3]Final Biomass EFs'!$A$22:$A$26,0))*INDEX([4]BC_calcs!$D$86:$Q$86,1,MATCH($A76,[4]BC_calcs!$D$55:$Q$55,0))</f>
         <v>0.18125489675062256</v>
       </c>
       <c r="C76" s="24">
-        <f>INDEX('[1]Final Biomass EFs'!$K$48:$K$52,MATCH($A76,'[1]Final Biomass EFs'!$A$48:$A$52,0))*INDEX([2]OC_calcs!$D$88:$Q$88,1,MATCH($A76,[2]OC_calcs!$D$56:$Q$56,0))</f>
+        <f>INDEX('[3]Final Biomass EFs'!$K$48:$K$52,MATCH($A76,'[3]Final Biomass EFs'!$A$48:$A$52,0))*INDEX([4]OC_calcs!$D$88:$Q$88,1,MATCH($A76,[4]OC_calcs!$D$56:$Q$56,0))</f>
         <v>0.66068439918421884</v>
       </c>
       <c r="D76" s="20"/>
@@ -3774,37 +3803,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15:G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="16384" width="9.1640625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A1" s="27" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="14">
+    <row r="2" spans="1:19" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A3" s="29" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="13" thickBot="1">
+    <row r="4" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="29"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A5" s="30" t="s">
         <v>97</v>
       </c>
@@ -3827,7 +3856,7 @@
       <c r="R5" s="31"/>
       <c r="S5" s="32"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A6" s="33" t="s">
         <v>0</v>
       </c>
@@ -3850,7 +3879,7 @@
       <c r="R6" s="34"/>
       <c r="S6" s="35"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A7" s="33" t="s">
         <v>1</v>
       </c>
@@ -3873,7 +3902,7 @@
       <c r="R7" s="34"/>
       <c r="S7" s="35"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A8" s="33" t="s">
         <v>2</v>
       </c>
@@ -3896,7 +3925,7 @@
       <c r="R8" s="34"/>
       <c r="S8" s="35"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A9" s="33" t="s">
         <v>3</v>
       </c>
@@ -3919,7 +3948,7 @@
       <c r="R9" s="34"/>
       <c r="S9" s="35"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A10" s="33" t="s">
         <v>4</v>
       </c>
@@ -3942,7 +3971,7 @@
       <c r="R10" s="34"/>
       <c r="S10" s="35"/>
     </row>
-    <row r="11" spans="1:19" ht="13" thickBot="1">
+    <row r="11" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>5</v>
       </c>
@@ -3965,19 +3994,22 @@
       <c r="R11" s="37"/>
       <c r="S11" s="38"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A13" s="28" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="15">
+    <row r="15" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="39"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47" t="s">
+      <c r="F15" s="45"/>
+      <c r="G15" s="45" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="16" spans="1:19">
+      <c r="I15" s="28" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
@@ -3987,47 +4019,62 @@
       <c r="C16" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="47" t="s">
+      <c r="F16" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="G16" s="47">
+      <c r="G16" s="45">
         <f>1/A18</f>
         <v>0.32959789057350036</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="42" t="s">
+      <c r="I16" s="46">
+        <f>G16*42</f>
+        <v>13.843111404087015</v>
+      </c>
+      <c r="K16" s="49" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A17" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="43"/>
+      <c r="B17" s="48"/>
       <c r="C17" s="41"/>
-      <c r="F17" s="47" t="s">
+      <c r="F17" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="47">
+      <c r="G17" s="45">
         <f>1/B18</f>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="44">
+      <c r="I17" s="46">
+        <f t="shared" ref="I17:I18" si="0">G17*42</f>
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A18" s="42">
         <v>3.0339999999999998</v>
       </c>
-      <c r="B18" s="45">
+      <c r="B18" s="43">
         <v>5</v>
       </c>
-      <c r="C18" s="45">
+      <c r="C18" s="43">
         <v>0.68</v>
       </c>
-      <c r="F18" s="47" t="s">
+      <c r="F18" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="47">
+      <c r="G18" s="45">
         <f>1/C18</f>
         <v>1.4705882352941175</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="14">
+      <c r="I18" s="46">
+        <f t="shared" si="0"/>
+        <v>61.764705882352935</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -4035,8 +4082,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14">
-      <c r="B21" s="46" t="s">
+    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="B21" s="44" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4056,20 +4103,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.5" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -4086,7 +4133,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -4097,14 +4144,14 @@
         <v>29</v>
       </c>
       <c r="D2">
-        <f>'Biofuels_9.xls'!G17</f>
+        <f>Biofuels_9.xls!G17</f>
         <v>0.2</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -4115,14 +4162,14 @@
         <v>29</v>
       </c>
       <c r="D3">
-        <f>'Biofuels_9.xls'!G17</f>
+        <f>Biofuels_9.xls!G17</f>
         <v>0.2</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -4133,14 +4180,14 @@
         <v>29</v>
       </c>
       <c r="D4">
-        <f>'Biofuels_9.xls'!G18</f>
+        <f>Biofuels_9.xls!G18</f>
         <v>1.4705882352941175</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -4151,14 +4198,14 @@
         <v>29</v>
       </c>
       <c r="D5">
-        <f>'Biofuels_9.xls'!G18</f>
+        <f>Biofuels_9.xls!G18</f>
         <v>1.4705882352941175</v>
       </c>
       <c r="E5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -4169,14 +4216,14 @@
         <v>29</v>
       </c>
       <c r="D6">
-        <f>'Biofuels_9.xls'!G16</f>
+        <f>Biofuels_9.xls!G16</f>
         <v>0.32959789057350036</v>
       </c>
       <c r="E6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -4195,7 +4242,7 @@
         <v>Fernandes et al (2007)</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -4207,14 +4254,14 @@
       </c>
       <c r="D8">
         <f>'Bio EF Calcs.xlsx'!K4</f>
-        <v>0.32244196044712498</v>
+        <v>0.3214285714285714</v>
       </c>
       <c r="E8" t="str">
         <f>'Bio EF Calcs.xlsx'!F4</f>
         <v>Yevich &amp; Logan 2002</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -4226,14 +4273,14 @@
       </c>
       <c r="D9">
         <f>'Bio EF Calcs.xlsx'!K4</f>
-        <v>0.32244196044712498</v>
+        <v>0.3214285714285714</v>
       </c>
       <c r="E9" t="str">
         <f>'Bio EF Calcs.xlsx'!F4</f>
         <v>Yevich &amp; Logan 2002</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -4245,14 +4292,14 @@
       </c>
       <c r="D10">
         <f>'Bio EF Calcs.xlsx'!K5</f>
-        <v>0.34632655010987501</v>
+        <v>0.34523809523809523</v>
       </c>
       <c r="E10" t="str">
         <f>'Bio EF Calcs.xlsx'!F5</f>
         <v>Yevich &amp; Logan 2002</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>26</v>
       </c>

</xml_diff>